<commit_message>
three level all results
</commit_message>
<xml_diff>
--- a/Results/Three Level Numbers.xlsx
+++ b/Results/Three Level Numbers.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Min Preprocessing</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Tf-Idf</t>
+  </si>
+  <si>
+    <t>Using LR, one hot encoding and ngram(1,2)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,15 +666,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
@@ -679,206 +682,239 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="7">
-        <v>3114</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1003</v>
-      </c>
-      <c r="D2" s="7">
-        <v>95.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7">
-        <v>438</v>
-      </c>
-      <c r="C3" s="7">
-        <v>137</v>
-      </c>
-      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7">
-        <v>873</v>
+        <v>3114</v>
       </c>
       <c r="C4" s="7">
-        <v>279</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>1003</v>
+      </c>
+      <c r="D4" s="7">
+        <v>95.2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7">
-        <v>102</v>
+        <v>438</v>
       </c>
       <c r="C5" s="7">
-        <v>39</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="D5" s="7">
+        <v>94.8</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7">
-        <v>5270</v>
+        <v>873</v>
       </c>
       <c r="C6" s="7">
-        <v>1699</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>279</v>
+      </c>
+      <c r="D6" s="7">
+        <v>86.7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7">
-        <v>571</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7">
-        <v>348</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="D7" s="7">
+        <v>89.7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7">
-        <v>312</v>
+        <v>5270</v>
       </c>
       <c r="C8" s="7">
-        <v>107</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>1699</v>
+      </c>
+      <c r="D8" s="7">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7">
+        <v>571</v>
+      </c>
+      <c r="C9" s="7">
+        <v>348</v>
+      </c>
+      <c r="D9" s="7">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7">
+        <v>312</v>
+      </c>
+      <c r="C10" s="7">
+        <v>107</v>
+      </c>
+      <c r="D10" s="7">
+        <v>89.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B11" s="7">
         <v>544</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C11" s="7">
         <v>175</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="9">
-        <v>3552</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1140</v>
-      </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="7">
+        <v>93.7</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="9">
-        <v>4425</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1419</v>
-      </c>
-      <c r="D12" s="9"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="9">
-        <v>4527</v>
+        <v>3552</v>
       </c>
       <c r="C13" s="9">
-        <v>1458</v>
-      </c>
-      <c r="D13" s="9"/>
+        <v>1140</v>
+      </c>
+      <c r="D13" s="9">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>9797</v>
+        <v>4425</v>
       </c>
       <c r="C14" s="9">
-        <v>3157</v>
-      </c>
-      <c r="D14" s="9"/>
+        <v>1419</v>
+      </c>
+      <c r="D14" s="9">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="9">
-        <v>10368</v>
+        <v>4527</v>
       </c>
       <c r="C15" s="9">
-        <v>3505</v>
-      </c>
-      <c r="D15" s="9"/>
+        <v>1458</v>
+      </c>
+      <c r="D15" s="9">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="9">
-        <v>10680</v>
+        <v>9797</v>
       </c>
       <c r="C16" s="9">
-        <v>3612</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>3157</v>
+      </c>
+      <c r="D16" s="9">
+        <v>93.7</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9">
+        <v>10368</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3505</v>
+      </c>
+      <c r="D17" s="9">
+        <v>94.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="9">
+        <v>10680</v>
+      </c>
+      <c r="C18" s="9">
+        <v>3612</v>
+      </c>
+      <c r="D18" s="9">
+        <v>93.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B19" s="9">
         <v>11224</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C19" s="9">
         <v>3787</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D19" s="9">
+        <v>94.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
two level all results
</commit_message>
<xml_diff>
--- a/Results/Three Level Numbers.xlsx
+++ b/Results/Three Level Numbers.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Min Preprocessing</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Tf-Idf</t>
+  </si>
+  <si>
+    <t>Using LR, one hot encoding and ngram(1,2)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,15 +666,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
@@ -679,206 +682,239 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="7">
-        <v>3114</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1003</v>
-      </c>
-      <c r="D2" s="7">
-        <v>95.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7">
-        <v>438</v>
-      </c>
-      <c r="C3" s="7">
-        <v>137</v>
-      </c>
-      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7">
-        <v>873</v>
+        <v>3114</v>
       </c>
       <c r="C4" s="7">
-        <v>279</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>1003</v>
+      </c>
+      <c r="D4" s="7">
+        <v>95.2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7">
-        <v>102</v>
+        <v>438</v>
       </c>
       <c r="C5" s="7">
-        <v>39</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="D5" s="7">
+        <v>94.8</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7">
-        <v>5270</v>
+        <v>873</v>
       </c>
       <c r="C6" s="7">
-        <v>1699</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>279</v>
+      </c>
+      <c r="D6" s="7">
+        <v>86.7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7">
-        <v>571</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7">
-        <v>348</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="D7" s="7">
+        <v>89.7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7">
-        <v>312</v>
+        <v>5270</v>
       </c>
       <c r="C8" s="7">
-        <v>107</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>1699</v>
+      </c>
+      <c r="D8" s="7">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7">
+        <v>571</v>
+      </c>
+      <c r="C9" s="7">
+        <v>348</v>
+      </c>
+      <c r="D9" s="7">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7">
+        <v>312</v>
+      </c>
+      <c r="C10" s="7">
+        <v>107</v>
+      </c>
+      <c r="D10" s="7">
+        <v>89.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B11" s="7">
         <v>544</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C11" s="7">
         <v>175</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="9">
-        <v>3552</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1140</v>
-      </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="7">
+        <v>93.7</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="9">
-        <v>4425</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1419</v>
-      </c>
-      <c r="D12" s="9"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="9">
-        <v>4527</v>
+        <v>3552</v>
       </c>
       <c r="C13" s="9">
-        <v>1458</v>
-      </c>
-      <c r="D13" s="9"/>
+        <v>1140</v>
+      </c>
+      <c r="D13" s="9">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>9797</v>
+        <v>4425</v>
       </c>
       <c r="C14" s="9">
-        <v>3157</v>
-      </c>
-      <c r="D14" s="9"/>
+        <v>1419</v>
+      </c>
+      <c r="D14" s="9">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="9">
-        <v>10368</v>
+        <v>4527</v>
       </c>
       <c r="C15" s="9">
-        <v>3505</v>
-      </c>
-      <c r="D15" s="9"/>
+        <v>1458</v>
+      </c>
+      <c r="D15" s="9">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="9">
-        <v>10680</v>
+        <v>9797</v>
       </c>
       <c r="C16" s="9">
-        <v>3612</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>3157</v>
+      </c>
+      <c r="D16" s="9">
+        <v>93.7</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9">
+        <v>10368</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3505</v>
+      </c>
+      <c r="D17" s="9">
+        <v>94.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="9">
+        <v>10680</v>
+      </c>
+      <c r="C18" s="9">
+        <v>3612</v>
+      </c>
+      <c r="D18" s="9">
+        <v>93.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B19" s="9">
         <v>11224</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C19" s="9">
         <v>3787</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D19" s="9">
+        <v>94.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>